<commit_message>
friedman first vis table
</commit_message>
<xml_diff>
--- a/inst/extdata/friedman_test.xlsx
+++ b/inst/extdata/friedman_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OMAR_2016\Github_Repos\iskay\inst\ext\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OMAR_2016\Github_Repos\iskay\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Jueces</t>
   </si>
@@ -36,6 +36,21 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>j1</t>
+  </si>
+  <si>
+    <t>j2</t>
+  </si>
+  <si>
+    <t>j3</t>
+  </si>
+  <si>
+    <t>j4</t>
+  </si>
+  <si>
+    <t>j5</t>
   </si>
 </sst>
 </file>
@@ -407,7 +422,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,8 +445,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -444,8 +459,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -458,8 +473,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -472,8 +487,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -486,8 +501,8 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -500,8 +515,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -514,8 +529,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -528,8 +543,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -542,8 +557,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>4</v>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -556,8 +571,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>5</v>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -570,8 +585,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -584,8 +599,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>2</v>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -598,8 +613,8 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
-        <v>3</v>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -612,8 +627,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
-        <v>4</v>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -626,8 +641,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
-        <v>5</v>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -640,8 +655,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -654,8 +669,8 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
-        <v>2</v>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -668,8 +683,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
-        <v>3</v>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -682,8 +697,8 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
-        <v>4</v>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="1">
         <v>4</v>
@@ -696,8 +711,8 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
-        <v>5</v>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>

</xml_diff>